<commit_message>
feat: JPA buscar por ID
</commit_message>
<xml_diff>
--- a/db/PRODUCTOS_DATA.xlsx
+++ b/db/PRODUCTOS_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andes\OneDrive\Documentos\NetBeansProjects\EcommerceADSO6_back\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grupologis\Documents\NetBeansProjects\EcommcerceADSO6_backend\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016AD4F7-CCDC-4EDF-BF80-70CA2D8371FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39349EE6-3D23-4E0A-B2E0-E2E90E621243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="156">
   <si>
     <t>id_producto</t>
   </si>
@@ -192,19 +192,307 @@
     <t>https://automatednow.com/images/detailed/3/Echo_Dot_4th_Gen_White_950_zyqo-ih.png</t>
   </si>
   <si>
-    <t>Impresora multifuncional</t>
-  </si>
-  <si>
-    <t>Dispositivo que imprime, escanea</t>
-  </si>
-  <si>
     <t>HP</t>
   </si>
   <si>
-    <t>OfficeJet Pro 9015</t>
-  </si>
-  <si>
-    <t>https://crdms.images.consumerreports.org/f_auto,w_600/prod/products/cr/models/398284-all-in-one-printers-hp-officejet-pro-9015-10007084.png</t>
+    <t>Auriculares inalámbricos con cancelación de ruido</t>
+  </si>
+  <si>
+    <t>Auriculares Bluetooth con tecnología de cancelación de ruido activa</t>
+  </si>
+  <si>
+    <t>2024-03-26 00:00:00.000</t>
+  </si>
+  <si>
+    <t>Tablet con pantalla táctil de 10 pulgadas</t>
+  </si>
+  <si>
+    <t>Tablet con pantalla Retina de 10.9 pulgadas y chip A14 Bionic</t>
+  </si>
+  <si>
+    <t>iPad Air (2022)</t>
+  </si>
+  <si>
+    <t>Cámara digital con sensor de 24 megapíxeles</t>
+  </si>
+  <si>
+    <t>Cámara DSLR con sensor CMOS de formato completo y grabación de video 8K</t>
+  </si>
+  <si>
+    <t>EOS R5</t>
+  </si>
+  <si>
+    <t>Reloj inteligente con monitor de frecuencia cardíaca</t>
+  </si>
+  <si>
+    <t>Reloj deportivo con GPS y resistencia al agua</t>
+  </si>
+  <si>
+    <t>Garmin</t>
+  </si>
+  <si>
+    <t>Forerunner 945</t>
+  </si>
+  <si>
+    <t>Altavoz Bluetooth portátil resistente al agua</t>
+  </si>
+  <si>
+    <t>Altavoz inalámbrico con batería de larga duración</t>
+  </si>
+  <si>
+    <t>JBL</t>
+  </si>
+  <si>
+    <t>Charge 5</t>
+  </si>
+  <si>
+    <t>Impresora multifunción con conectividad Wi-Fi</t>
+  </si>
+  <si>
+    <t>Impresora láser con escáner y copiadora integrados</t>
+  </si>
+  <si>
+    <t>LaserJet Pro MFP M227fdw</t>
+  </si>
+  <si>
+    <t>Mochila para portátil de 15 pulgadas con puerto USB</t>
+  </si>
+  <si>
+    <t>Mochila resistente al agua con compartimento acolchado para laptop</t>
+  </si>
+  <si>
+    <t>SwissGear</t>
+  </si>
+  <si>
+    <t>SA1923</t>
+  </si>
+  <si>
+    <t>Router Wi-Fi 6 de doble banda para redes domésticas</t>
+  </si>
+  <si>
+    <t>Router inalámbrico con tecnología MU-MIMO y velocidad de hasta 6000 Mbps</t>
+  </si>
+  <si>
+    <t>TP-Link</t>
+  </si>
+  <si>
+    <t>Archer AX6000</t>
+  </si>
+  <si>
+    <t>Monitor de 27 pulgadas con resolución 4K y HDR</t>
+  </si>
+  <si>
+    <t>Monitor IPS con frecuencia de actualización de 144Hz y tiempo de respuesta de 1ms</t>
+  </si>
+  <si>
+    <t>27UL850-W</t>
+  </si>
+  <si>
+    <t>Refrigerador de doble puerta con dispensador de agua</t>
+  </si>
+  <si>
+    <t>Refrigerador de acero inoxidable con sistema de enfriamiento inteligente</t>
+  </si>
+  <si>
+    <t>RF27T5501SG</t>
+  </si>
+  <si>
+    <t>Aspiradora robot con mapeo inteligente de la casa</t>
+  </si>
+  <si>
+    <t>Aspiradora automática con tecnología de navegación láser</t>
+  </si>
+  <si>
+    <t>iRobot</t>
+  </si>
+  <si>
+    <t>Roomba i7+</t>
+  </si>
+  <si>
+    <t>Silla de escritorio ergonómica con soporte lumbar</t>
+  </si>
+  <si>
+    <t>Silla de oficina ajustable con reposabrazos y respaldo reclinable</t>
+  </si>
+  <si>
+    <t>Herman Miller</t>
+  </si>
+  <si>
+    <t>Aeron Remastered</t>
+  </si>
+  <si>
+    <t>Batería externa de 20000 mAh con carga rápida</t>
+  </si>
+  <si>
+    <t>Powerbank con puerto USB-C y tecnología de carga rápida Power Delivery</t>
+  </si>
+  <si>
+    <t>Anker</t>
+  </si>
+  <si>
+    <t>PowerCore+ 26800 PD</t>
+  </si>
+  <si>
+    <t>Horno eléctrico con función de convección y grill</t>
+  </si>
+  <si>
+    <t>Horno empotrable con capacidad de 60 litros y control digital</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>HBG675BB1</t>
+  </si>
+  <si>
+    <t>Máquina de café automática con molinillo integrado</t>
+  </si>
+  <si>
+    <t>Cafetera espresso con sistema de preparación de leche automático</t>
+  </si>
+  <si>
+    <t>De'Longhi</t>
+  </si>
+  <si>
+    <t>Magnifica S</t>
+  </si>
+  <si>
+    <t>Barra de sonido Dolby Atmos con subwoofer inalámbrico</t>
+  </si>
+  <si>
+    <t>Sistema de audio envolvente con tecnología de audio 3D</t>
+  </si>
+  <si>
+    <t>HT-G700</t>
+  </si>
+  <si>
+    <t>Cortadora de césped eléctrica con batería recargable</t>
+  </si>
+  <si>
+    <t>Cortacésped inalámbrico con ajuste de altura de corte</t>
+  </si>
+  <si>
+    <t>Greenworks</t>
+  </si>
+  <si>
+    <t>Pro 80V</t>
+  </si>
+  <si>
+    <t>Lámpara de escritorio LED con control táctil</t>
+  </si>
+  <si>
+    <t>Lámpara de mesa regulable con puerto de carga USB</t>
+  </si>
+  <si>
+    <t>TaoTronics</t>
+  </si>
+  <si>
+    <t>TT-DL13</t>
+  </si>
+  <si>
+    <t>Cocina de inducción con cuatro quemadores y control táctil</t>
+  </si>
+  <si>
+    <t>Placa de cocina con función de bloqueo de seguridad y temporizador</t>
+  </si>
+  <si>
+    <t>Beko</t>
+  </si>
+  <si>
+    <t>HII64400AT</t>
+  </si>
+  <si>
+    <t>Smartwatch deportivo con seguimiento de actividad física</t>
+  </si>
+  <si>
+    <t>Reloj inteligente con monitor de sueño y resistencia al agua</t>
+  </si>
+  <si>
+    <t>Licuadora de alta potencia con vaso de vidrio</t>
+  </si>
+  <si>
+    <t>Batidora con motor de 1200W y cuchillas de acero inoxidable</t>
+  </si>
+  <si>
+    <t>Oster</t>
+  </si>
+  <si>
+    <t>BRLY07-Z00-050</t>
+  </si>
+  <si>
+    <t>Cámara de seguridad para exteriores con visión nocturna</t>
+  </si>
+  <si>
+    <t>Cámara IP resistente a la intemperie con detección de movimiento</t>
+  </si>
+  <si>
+    <t>Arlo</t>
+  </si>
+  <si>
+    <t>Pro 4</t>
+  </si>
+  <si>
+    <t>https://cosonyb2c.vtexassets.com/arquivos/ids/352765/wh1000xm4L-1.jpg?v=637673971750170000</t>
+  </si>
+  <si>
+    <t>https://www.att.com/scmsassets/global/devices/tablets/apple/apple-ipad-air-5th-gen-_2022_/carousel/purple/Purple-1.png</t>
+  </si>
+  <si>
+    <t>https://i1.adis.ws/i/canon/eos-r5_front_rf24-105mmf4lisusm_32c26ad194234d42b3cd9e582a21c99b</t>
+  </si>
+  <si>
+    <t>https://ph.garmin.com/m/ph/g/products/Forerunner945-black-image-01.png</t>
+  </si>
+  <si>
+    <t>https://www.jbl.com.co/dw/image/v2/AAUJ_PRD/on/demandware.static/-/Sites-masterCatalog_Harman/default/dw68c39957/JBL_CHARGE5_WIFI_HERO%20_LEFT_37890_x3.png?sw=537&amp;sfrm=png</t>
+  </si>
+  <si>
+    <t>https://ssl-product-images.www8-hp.com/digmedialib/prodimg/lowres/c05288908.png</t>
+  </si>
+  <si>
+    <t>https://tottoco.vteximg.com.br/arquivos/ids/161247-292-292/SKYNET-1320G-N01_A.png?v=636472200715300000</t>
+  </si>
+  <si>
+    <t>https://tecnokefren.com/wp-content/uploads/2021/08/ARCHERAX6000-h.png</t>
+  </si>
+  <si>
+    <t>https://media.croma.com/image/upload/v1683209601/Croma%20Assets/Computers%20Peripherals/Monitor/Images/263397_4_i6saea.png</t>
+  </si>
+  <si>
+    <t>https://images.samsung.com/is/image/samsung/mx-french-door-rf27t5501sg-rf27t5501sg-em-frontblack-thumb-299315752</t>
+  </si>
+  <si>
+    <t>https://res-2.cloudinary.com/grover/image/upload/v1686582235/mf8wd8wz0cv5t9l1cu33.png</t>
+  </si>
+  <si>
+    <t>https://newstar.sg/cdn/shop/products/WhatsApp_Image_2021-08-02_at_12.26.31_PM-removebg-preview_1024x1024.png?v=1709690975</t>
+  </si>
+  <si>
+    <t>https://shareefcorner.sa/pub/media/catalog/product/cache/82d05cd6abfc8fcfb8bdbf5accf96e1b/b/1/b1376k11_1__1.png</t>
+  </si>
+  <si>
+    <t>https://media3.bosch-home.com/Product_Shots/1600x900/MCSA00766727_411060_HBG672BB1F_def.png</t>
+  </si>
+  <si>
+    <t>https://assets.mmsrg.com/isr/166325/c1/-/ASSET_MMS_96585590/fee_786_587_png</t>
+  </si>
+  <si>
+    <t>https://www.sony.co.in/image/e6b1cb62d9484aabfe6bebdbd0fa5709?fmt=png-alpha&amp;wid=900&amp;hei=800</t>
+  </si>
+  <si>
+    <t>https://greenworkstools.ca/cdn/shop/files/4_06bdf49d-7138-4217-8835-806cc2423989_800x.png?v=1712168690</t>
+  </si>
+  <si>
+    <t>https://bluetek.co.za/wp-content/uploads/2021/11/TT-DL13-B_2.png</t>
+  </si>
+  <si>
+    <t>https://www.beko.com/content/dam/germany-de-aem/germany-de-aemProductCatalog/product-images/7757182903-HII-64400-AT/7757182903-LO1-20140909-131553.png/jcr:content/renditions/cq5dam.web.1280.1280.png</t>
+  </si>
+  <si>
+    <t>https://s13emagst.akamaized.net/products/67066/67065104/images/res_8f597c6b37a932ba89cbdc5e326bba6a.png?width=300&amp;height=300&amp;hash=DF68DFF4C1B4B40940E84B247239BCEC</t>
+  </si>
+  <si>
+    <t>https://www1.djicdn.com/dps/645555df83f504bb5375e7e962aac9f0.webp</t>
   </si>
 </sst>
 </file>
@@ -525,27 +813,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="82.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="135" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="201.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="58.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="23.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,9 +863,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -603,9 +892,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -632,9 +921,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
@@ -661,9 +950,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>25</v>
@@ -690,9 +979,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>30</v>
@@ -719,9 +1008,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
@@ -748,9 +1037,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>40</v>
@@ -777,9 +1066,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>45</v>
@@ -806,9 +1095,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>50</v>
@@ -835,33 +1124,642 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="1">
+        <v>349990</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1">
+        <v>699990</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2799990</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="1">
+        <v>549990</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="1">
+        <v>199990</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="1">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F11" s="1">
-        <v>199990</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="1">
-        <v>10</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>59</v>
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1">
+        <v>269990</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="1">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="1">
+        <v>79990</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="1">
+        <v>499990</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1">
+        <v>3</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>20</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="1">
+        <v>499990</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1999990</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="1">
+        <v>899990</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="1">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>23</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1199990</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1">
+        <v>89990</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="1">
+        <v>399990</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="1">
+        <v>449990</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="1">
+        <v>599990</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F27" s="1">
+        <v>279990</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>29</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" s="1">
+        <v>29990</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="1">
+        <v>219990</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>31</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" s="1">
+        <v>349990</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="1">
+        <v>3</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>32</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="1">
+        <v>79990</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>33</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="1">
+        <v>349990</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="1">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>